<commit_message>
Updating system requirements and checking ADRs
</commit_message>
<xml_diff>
--- a/Requirements/System Requirements/System Requirements.xlsx
+++ b/Requirements/System Requirements/System Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shari\Documents\GitHub\Hey-Blue\Requirements\System Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACB72DB-E0DF-428E-82E7-AB9920B9C837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7325F3-1417-447B-9613-F63F0BADA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1030" yWindow="1070" windowWidth="15590" windowHeight="7780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System Requirements (RQ)" sheetId="2" r:id="rId1"/>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Requirements tracking added PKs
</commit_message>
<xml_diff>
--- a/Requirements/System Requirements/System Requirements.xlsx
+++ b/Requirements/System Requirements/System Requirements.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shari\Documents\GitHub\Hey-Blue\Requirements\System Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7325F3-1417-447B-9613-F63F0BADA369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45F6C7C-416C-46F7-B4AA-B079312451CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1030" yWindow="1070" windowWidth="15590" windowHeight="7780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System Requirements (RQ)" sheetId="2" r:id="rId1"/>
+    <sheet name="User Stories (US)" sheetId="3" r:id="rId2"/>
+    <sheet name="Archived Notes" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="134">
   <si>
     <t>Web and Mobile-Based with back-end processing and reporting and analytics that tracks site activity, connections</t>
   </si>
@@ -225,6 +227,216 @@
   </si>
   <si>
     <t>SR-MM-002</t>
+  </si>
+  <si>
+    <t>Criticality</t>
+  </si>
+  <si>
+    <t>US-001</t>
+  </si>
+  <si>
+    <t>Creating an Interaction</t>
+  </si>
+  <si>
+    <t>Police Officer Donate Points</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Notify Proximity</t>
+  </si>
+  <si>
+    <t>Interact</t>
+  </si>
+  <si>
+    <t>Earn Points</t>
+  </si>
+  <si>
+    <t>Share on social media</t>
+  </si>
+  <si>
+    <t>Browse Store</t>
+  </si>
+  <si>
+    <t>Redeem Points</t>
+  </si>
+  <si>
+    <t>Browse Charity</t>
+  </si>
+  <si>
+    <t>Donate Points</t>
+  </si>
+  <si>
+    <t>Send to Analytics</t>
+  </si>
+  <si>
+    <t>US-002</t>
+  </si>
+  <si>
+    <t>US-003</t>
+  </si>
+  <si>
+    <t>US-004</t>
+  </si>
+  <si>
+    <t>US-005</t>
+  </si>
+  <si>
+    <t>US-006</t>
+  </si>
+  <si>
+    <t>US-007</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>E-Commerce</t>
+  </si>
+  <si>
+    <t>Retailers register</t>
+  </si>
+  <si>
+    <t>Charity registers</t>
+  </si>
+  <si>
+    <t>Manage retailers offerings</t>
+  </si>
+  <si>
+    <t>Maintain charity store front</t>
+  </si>
+  <si>
+    <t>Present metrics and reporting</t>
+  </si>
+  <si>
+    <t>US-008</t>
+  </si>
+  <si>
+    <t>US-009</t>
+  </si>
+  <si>
+    <t>US-010</t>
+  </si>
+  <si>
+    <t>US-011</t>
+  </si>
+  <si>
+    <t>US-012</t>
+  </si>
+  <si>
+    <t>US-013</t>
+  </si>
+  <si>
+    <t>US-014</t>
+  </si>
+  <si>
+    <t>US-015</t>
+  </si>
+  <si>
+    <t>Web and Mobile-Based</t>
+  </si>
+  <si>
+    <t>End-Use Ease of Use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Officers location auto shut off </t>
+  </si>
+  <si>
+    <t>Officers cannot find citizens</t>
+  </si>
+  <si>
+    <t>No direct location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The App must protect user data </t>
+  </si>
+  <si>
+    <t>Allow Civilians to redeem points</t>
+  </si>
+  <si>
+    <t>Allow Officers to donate points</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store catalog of items </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offer points for fines/fees </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track how the points were used </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Track engagement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upload to social media </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3rd parties to create a storefront </t>
+  </si>
+  <si>
+    <t>Track officer connections</t>
+  </si>
+  <si>
+    <t>Single device to an email address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opt in &amp; out of push notifications </t>
+  </si>
+  <si>
+    <t>Aggregate data for impact report</t>
+  </si>
+  <si>
+    <t>1 connection per officer per day</t>
+  </si>
+  <si>
+    <t>Connectivity to Social Media</t>
+  </si>
+  <si>
+    <t>Software Systems (SS)</t>
+  </si>
+  <si>
+    <t>SS-001</t>
+  </si>
+  <si>
+    <t>Interaction Manager</t>
+  </si>
+  <si>
+    <t>Media Manager</t>
+  </si>
+  <si>
+    <t>Analytics &amp; Reporting</t>
+  </si>
+  <si>
+    <t>Donation &amp; Redemption</t>
+  </si>
+  <si>
+    <t>SS-002</t>
+  </si>
+  <si>
+    <t>SS-003</t>
+  </si>
+  <si>
+    <t>SS-004</t>
+  </si>
+  <si>
+    <t>Architectural Style</t>
+  </si>
+  <si>
+    <t>Architectural Characteristics</t>
+  </si>
+  <si>
+    <t>Architectural Principles</t>
+  </si>
+  <si>
+    <t>Architectural Decision Types</t>
+  </si>
+  <si>
+    <t>Functional High Level</t>
+  </si>
+  <si>
+    <t>Functional Details</t>
   </si>
 </sst>
 </file>
@@ -240,29 +452,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,6 +483,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -316,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -330,13 +547,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -655,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:C17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,12 +882,14 @@
     <col min="3" max="3" width="94.26953125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1"/>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -698,12 +916,14 @@
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5"/>
-      <c r="B5" s="5" t="s">
+    <row r="5" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -814,12 +1034,14 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17"/>
+    <row r="17" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="B17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
@@ -917,12 +1139,14 @@
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28"/>
+    <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="B28" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
@@ -987,12 +1211,14 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36"/>
+    <row r="36" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>64</v>
+      </c>
       <c r="B36" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
@@ -1022,7 +1248,491 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B36:C36"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6414F3B-3A24-4842-ABF7-E998B0CCEC45}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="31.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A23:B23"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAAF0ED-248C-45A0-B476-97ECE9241F16}">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33:D38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="29.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="8"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="8"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D33" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D34" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D35" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D36" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D37" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D38" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A28:B28"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Id to all artifacts
</commit_message>
<xml_diff>
--- a/Requirements/System Requirements/System Requirements.xlsx
+++ b/Requirements/System Requirements/System Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shari\Documents\GitHub\Hey-Blue\Requirements\System Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45F6C7C-416C-46F7-B4AA-B079312451CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A98B2D-430D-4163-983D-17F2E0776F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System Requirements (RQ)" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="136">
   <si>
     <t>Web and Mobile-Based with back-end processing and reporting and analytics that tracks site activity, connections</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Retailers register</t>
   </si>
   <si>
-    <t>Charity registers</t>
-  </si>
-  <si>
     <t>Manage retailers offerings</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
     <t xml:space="preserve">Track how the points were used </t>
   </si>
   <si>
-    <t xml:space="preserve">Track engagement </t>
-  </si>
-  <si>
     <t xml:space="preserve">Upload to social media </t>
   </si>
   <si>
@@ -437,13 +431,38 @@
   </si>
   <si>
     <t>Functional Details</t>
+  </si>
+  <si>
+    <t>SR-IM-011</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">EU Regulation, ability to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>delete profile</t>
+    </r>
+  </si>
+  <si>
+    <t>Delete profile and user data</t>
+  </si>
+  <si>
+    <t>3rd Party Registers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,8 +491,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,8 +519,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEEF0A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8F0A2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA2D4F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6D7C2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -529,11 +580,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -555,12 +617,29 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF6D7C2"/>
+      <color rgb="FFA2D4F0"/>
+      <color rgb="FFB8F0A2"/>
+      <color rgb="FFEEF0A2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -869,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -944,7 +1023,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -955,7 +1034,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -966,7 +1045,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -977,36 +1056,38 @@
         <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="B11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1015,54 +1096,52 @@
         <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
         <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="8"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1070,10 +1149,10 @@
         <v>56</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1081,10 +1160,10 @@
         <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1092,98 +1171,98 @@
         <v>56</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1191,62 +1270,73 @@
         <v>56</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C34" s="3" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="2"/>
-      <c r="B34" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
+      <c r="B35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="2"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C36" s="8"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="C37" s="8"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="2"/>
-      <c r="B38" s="3" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="2"/>
+      <c r="B39" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1256,10 +1346,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6414F3B-3A24-4842-ABF7-E998B0CCEC45}">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,7 +1433,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>73</v>
@@ -1351,7 +1441,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>74</v>
@@ -1365,7 +1455,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>77</v>
@@ -1373,37 +1463,37 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="12"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>96</v>
-      </c>
       <c r="B18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>86</v>
@@ -1411,53 +1501,57 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>124</v>
-      </c>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1468,8 +1562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAAF0ED-248C-45A0-B476-97ECE9241F16}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="A1:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1490,7 +1584,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -1498,7 +1592,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1516,7 +1610,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1524,7 +1618,7 @@
         <v>23</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1540,7 +1634,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -1548,7 +1642,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1556,7 +1650,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -1564,107 +1658,107 @@
         <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="7" t="s">
+      <c r="B14" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>105</v>
-      </c>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
+      <c r="B21" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>116</v>
-      </c>
+      <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1682,7 +1776,7 @@
         <v>62</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1690,45 +1784,45 @@
         <v>63</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D33" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D34" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D35" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D36" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D37" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D38" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A28:B28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
reviewing requirements and adrs
</commit_message>
<xml_diff>
--- a/Requirements/System Requirements/System Requirements.xlsx
+++ b/Requirements/System Requirements/System Requirements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shari\Documents\GitHub\Hey-Blue\Requirements\System Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A98B2D-430D-4163-983D-17F2E0776F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB6684A-2780-47FE-B554-063CF32AE252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="190" yWindow="230" windowWidth="17670" windowHeight="9550" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System Requirements (RQ)" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="139">
   <si>
     <t>Web and Mobile-Based with back-end processing and reporting and analytics that tracks site activity, connections</t>
   </si>
@@ -241,9 +241,6 @@
     <t>Police Officer Donate Points</t>
   </si>
   <si>
-    <t>Register</t>
-  </si>
-  <si>
     <t>Notify Proximity</t>
   </si>
   <si>
@@ -268,9 +265,6 @@
     <t>Donate Points</t>
   </si>
   <si>
-    <t>Send to Analytics</t>
-  </si>
-  <si>
     <t>US-002</t>
   </si>
   <si>
@@ -292,21 +286,6 @@
     <t>Analytics</t>
   </si>
   <si>
-    <t>E-Commerce</t>
-  </si>
-  <si>
-    <t>Retailers register</t>
-  </si>
-  <si>
-    <t>Manage retailers offerings</t>
-  </si>
-  <si>
-    <t>Maintain charity store front</t>
-  </si>
-  <si>
-    <t>Present metrics and reporting</t>
-  </si>
-  <si>
     <t>US-008</t>
   </si>
   <si>
@@ -316,19 +295,7 @@
     <t>US-010</t>
   </si>
   <si>
-    <t>US-011</t>
-  </si>
-  <si>
     <t>US-012</t>
-  </si>
-  <si>
-    <t>US-013</t>
-  </si>
-  <si>
-    <t>US-014</t>
-  </si>
-  <si>
-    <t>US-015</t>
   </si>
   <si>
     <t>Web and Mobile-Based</t>
@@ -455,14 +422,56 @@
     <t>Delete profile and user data</t>
   </si>
   <si>
-    <t>3rd Party Registers</t>
+    <t>Register 3rd Party</t>
+  </si>
+  <si>
+    <t>Donate &amp; Redeem</t>
+  </si>
+  <si>
+    <t>Register User</t>
+  </si>
+  <si>
+    <t>SR-001</t>
+  </si>
+  <si>
+    <t>SR-002</t>
+  </si>
+  <si>
+    <t>SR-003</t>
+  </si>
+  <si>
+    <t>SR-004</t>
+  </si>
+  <si>
+    <t>SR-005</t>
+  </si>
+  <si>
+    <t>SR-007</t>
+  </si>
+  <si>
+    <t>SR-008</t>
+  </si>
+  <si>
+    <t>SR-009</t>
+  </si>
+  <si>
+    <t>SR-010</t>
+  </si>
+  <si>
+    <t>SR-006</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present metrics </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,8 +508,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -522,12 +544,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEEF0A2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8F0A2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -611,21 +627,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -950,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -965,10 +981,10 @@
       <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="8"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
@@ -999,10 +1015,10 @@
       <c r="A5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -1023,7 +1039,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1113,7 +1129,7 @@
         <v>56</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>4</v>
@@ -1128,10 +1144,10 @@
       <c r="A18" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
@@ -1233,10 +1249,10 @@
       <c r="A29" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2"/>
@@ -1305,10 +1321,10 @@
       <c r="A37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="8"/>
+      <c r="C37" s="9"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
@@ -1346,212 +1362,185 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6414F3B-3A24-4842-ABF7-E998B0CCEC45}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.08984375" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="B5" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+      <c r="B7" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B9" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="12"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>135</v>
+      <c r="A15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>88</v>
-      </c>
+      <c r="A18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="9"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
+      <c r="A25" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A16:B16"/>
+  <mergeCells count="5">
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1560,39 +1549,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BAAF0ED-248C-45A0-B476-97ECE9241F16}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="A1:B30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B30" sqref="A5:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" style="4" customWidth="1"/>
     <col min="2" max="2" width="29.36328125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -1600,30 +1589,30 @@
       <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>49</v>
@@ -1631,50 +1620,50 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>133</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>58</v>
+        <v>135</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -1682,49 +1671,49 @@
       <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>127</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>129</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>136</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1732,33 +1721,33 @@
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="8"/>
+      <c r="B23" s="9"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>43</v>
+        <v>130</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1766,55 +1755,55 @@
       <c r="B27" s="3"/>
     </row>
     <row r="28" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="9"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D33" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D34" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D35" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D36" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D37" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D38" s="3" t="s">
-        <v>131</v>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>